<commit_message>
why choose us section completed
</commit_message>
<xml_diff>
--- a/extras/responsive conversion.xlsx
+++ b/extras/responsive conversion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipe.lugo\Desktop\Dropbox\office.dropbox\portfolio\zap\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5C4F84-0466-42D2-9D32-C01535335BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0E5B76-717D-4D0E-8D69-D2091B4AA2AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17316" yWindow="-15492" windowWidth="16692" windowHeight="12264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26760" yWindow="-15288" windowWidth="6420" windowHeight="12684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
   <dimension ref="A1:E188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +736,7 @@
         <v>1.056rem</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20</v>
       </c>
@@ -752,7 +752,7 @@
         <v>1.111rem</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>21</v>
       </c>
@@ -768,7 +768,7 @@
         <v>1.167rem</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22</v>
       </c>
@@ -784,7 +784,7 @@
         <v>1.222rem</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>23</v>
       </c>
@@ -800,7 +800,7 @@
         <v>1.278rem</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
@@ -816,7 +816,7 @@
         <v>1.333rem</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>25</v>
       </c>
@@ -832,7 +832,7 @@
         <v>1.389rem</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>26</v>
       </c>
@@ -848,7 +848,7 @@
         <v>1.444rem</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>27</v>
       </c>
@@ -864,7 +864,7 @@
         <v>1.5rem</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>28</v>
       </c>
@@ -880,7 +880,7 @@
         <v>1.556rem</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>29</v>
       </c>
@@ -896,7 +896,7 @@
         <v>1.611rem</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>30</v>
       </c>
@@ -912,7 +912,7 @@
         <v>1.667rem</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>31</v>
       </c>
@@ -928,7 +928,7 @@
         <v>1.722rem</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>32</v>
       </c>
@@ -944,7 +944,7 @@
         <v>1.778rem</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>33</v>
       </c>
@@ -960,7 +960,7 @@
         <v>1.833rem</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>34</v>
       </c>
@@ -976,7 +976,7 @@
         <v>1.889rem</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>35</v>
       </c>
@@ -992,7 +992,7 @@
         <v>1.944rem</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>36</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>2rem</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>37</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>2.056rem</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>38</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>2.111rem</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>39</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>2.167rem</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>40</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>2.222rem</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>41</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>2.278rem</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>42</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>2.333rem</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>43</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>2.389rem</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>44</v>
       </c>

</xml_diff>